<commit_message>
Collaboration Part: Corrections according to Aslaks Feedback
</commit_message>
<xml_diff>
--- a/Report/images/collaboration/Milesstones.xlsx
+++ b/Report/images/collaboration/Milesstones.xlsx
@@ -431,10 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,8 +519,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="11" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="70" scale="84" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>